<commit_message>
3D Visualisation page complete
</commit_message>
<xml_diff>
--- a/public/Sound_and_3D_files/Participants_Info_Location.xlsx
+++ b/public/Sound_and_3D_files/Participants_Info_Location.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="167">
   <si>
     <t>name</t>
   </si>
@@ -28,6 +28,12 @@
     <t>stl</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>Colette Gribben</t>
   </si>
   <si>
@@ -37,6 +43,9 @@
     <t>Colette STL</t>
   </si>
   <si>
+    <t>important lady's daughter</t>
+  </si>
+  <si>
     <t>Justin C.</t>
   </si>
   <si>
@@ -46,6 +55,9 @@
     <t>Justin STL</t>
   </si>
   <si>
+    <t>considers sj their home</t>
+  </si>
+  <si>
     <t>Linda Poon</t>
   </si>
   <si>
@@ -55,6 +67,9 @@
     <t>Linda STL</t>
   </si>
   <si>
+    <t>community/veggielation</t>
+  </si>
+  <si>
     <t>Joshua Joya</t>
   </si>
   <si>
@@ -64,6 +79,9 @@
     <t>Joshua MP3</t>
   </si>
   <si>
+    <t>no description from this person</t>
+  </si>
+  <si>
     <t>Justin Slavick</t>
   </si>
   <si>
@@ -73,6 +91,9 @@
     <t>Justin S STL</t>
   </si>
   <si>
+    <t>Favorite annual SJ event</t>
+  </si>
+  <si>
     <t>William Garrett</t>
   </si>
   <si>
@@ -82,6 +103,9 @@
     <t>William STL</t>
   </si>
   <si>
+    <t>a story of him and his partner/yogurt run</t>
+  </si>
+  <si>
     <t>Michele</t>
   </si>
   <si>
@@ -91,18 +115,27 @@
     <t>Michele STL</t>
   </si>
   <si>
+    <t>story about a blue house</t>
+  </si>
+  <si>
     <t>Rosalyn</t>
   </si>
   <si>
     <t>Rosalyn STL</t>
   </si>
   <si>
+    <t>culture</t>
+  </si>
+  <si>
     <t>Arthur</t>
   </si>
   <si>
     <t>Arthur STL</t>
   </si>
   <si>
+    <t>city in search of its own personality</t>
+  </si>
+  <si>
     <t>James Bass</t>
   </si>
   <si>
@@ -112,6 +145,9 @@
     <t>James STL</t>
   </si>
   <si>
+    <t>SJ is one of the greatest cities</t>
+  </si>
+  <si>
     <t>Sean Paul Guess</t>
   </si>
   <si>
@@ -121,6 +157,9 @@
     <t>Sean STL</t>
   </si>
   <si>
+    <t>seeing the city's potential and</t>
+  </si>
+  <si>
     <t>Avery</t>
   </si>
   <si>
@@ -130,6 +169,9 @@
     <t>Avery STL</t>
   </si>
   <si>
+    <t xml:space="preserve">snappeas </t>
+  </si>
+  <si>
     <t>Toussaint Celestin</t>
   </si>
   <si>
@@ -139,12 +181,18 @@
     <t>Toussaint STL</t>
   </si>
   <si>
+    <t>memories of the ballpatk</t>
+  </si>
+  <si>
     <t>Elizabeth Agramont Justiniano</t>
   </si>
   <si>
     <t>Elizabeth STL</t>
   </si>
   <si>
+    <t>the community</t>
+  </si>
+  <si>
     <t>Galos &amp; Kostia</t>
   </si>
   <si>
@@ -154,6 +202,9 @@
     <t>Kostia STL</t>
   </si>
   <si>
+    <t xml:space="preserve">finding the cat and pick up their Majka </t>
+  </si>
+  <si>
     <t>is it San Jose Fountain Blues &amp; Brews Festival??</t>
   </si>
   <si>
@@ -163,12 +214,18 @@
     <t>David Duperrault</t>
   </si>
   <si>
+    <t>SJ has evolved from a home for indigenous to a magnet of immigrant farmers in the silicon valley</t>
+  </si>
+  <si>
     <t>Svavai Yeturi</t>
   </si>
   <si>
     <t>Svavai STL</t>
   </si>
   <si>
+    <t>the most happiest place in california</t>
+  </si>
+  <si>
     <t>Danielle</t>
   </si>
   <si>
@@ -178,6 +235,9 @@
     <t>Danielle.stl</t>
   </si>
   <si>
+    <t>Story between Danielle and Yoon</t>
+  </si>
+  <si>
     <t>Chetna</t>
   </si>
   <si>
@@ -187,6 +247,9 @@
     <t>chetna stl</t>
   </si>
   <si>
+    <t>making art for SJ Sharks for South Asian Heritage night</t>
+  </si>
+  <si>
     <t>Layla</t>
   </si>
   <si>
@@ -196,6 +259,9 @@
     <t>layla stl</t>
   </si>
   <si>
+    <t>lilies and how she likes the drinks at the event</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tristan </t>
   </si>
   <si>
@@ -205,6 +271,9 @@
     <t>tristan stl</t>
   </si>
   <si>
+    <t>living nearby and going for contact improv classes/few drinks</t>
+  </si>
+  <si>
     <t>Julius</t>
   </si>
   <si>
@@ -214,6 +283,9 @@
     <t>julius stl</t>
   </si>
   <si>
+    <t>their favorite spot being a grassy area with benches outside MLK lib.</t>
+  </si>
+  <si>
     <t>Tomás</t>
   </si>
   <si>
@@ -223,6 +295,9 @@
     <t>tomas stl</t>
   </si>
   <si>
+    <t>beginning of SJ graffiti art history</t>
+  </si>
+  <si>
     <t>Jessica</t>
   </si>
   <si>
@@ -232,6 +307,9 @@
     <t>jessica stl</t>
   </si>
   <si>
+    <t>the yummy Mexican food and their iconic orange sauce (handwriting didn't show up well on my camera)</t>
+  </si>
+  <si>
     <t>Seth (former BFA)</t>
   </si>
   <si>
@@ -241,12 +319,18 @@
     <t>seth stl</t>
   </si>
   <si>
+    <t>skateboarding and how he skateboarded here for 10+ years and how the stairs look smaller than he remembers</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hong </t>
   </si>
   <si>
     <t>hong stl</t>
   </si>
   <si>
+    <t>how I was born here and came back here for college and how I'm thankful for the opportunities here and starting fresh</t>
+  </si>
+  <si>
     <t>Mirae</t>
   </si>
   <si>
@@ -256,6 +340,9 @@
     <t>mirae stl</t>
   </si>
   <si>
+    <t>the bright colors of the low riders (very swaggy)</t>
+  </si>
+  <si>
     <t>Robert (former BFA)</t>
   </si>
   <si>
@@ -265,6 +352,9 @@
     <t>robert stl</t>
   </si>
   <si>
+    <t>how this is his favorite spot and that he made a lot of memories with the other BFA friends</t>
+  </si>
+  <si>
     <t>414 E William St suite a, San Jose, CA 95112?</t>
   </si>
   <si>
@@ -280,6 +370,9 @@
     <t>erin stl</t>
   </si>
   <si>
+    <t>a place how they grew professionally and grew up</t>
+  </si>
+  <si>
     <t>Kelvin (former BFA)</t>
   </si>
   <si>
@@ -289,6 +382,9 @@
     <t>kelvin stl</t>
   </si>
   <si>
+    <t>how san jose made him see that it is a diverse place and how he is grateful for the experiences</t>
+  </si>
+  <si>
     <t>Long (software dev)</t>
   </si>
   <si>
@@ -298,6 +394,9 @@
     <t>long stl</t>
   </si>
   <si>
+    <t>how he loves going on field trips to the tech museum as a kid</t>
+  </si>
+  <si>
     <t>Nia</t>
   </si>
   <si>
@@ -307,6 +406,9 @@
     <t>nia stl</t>
   </si>
   <si>
+    <t>she moved to SJ on a whim and how they came here after spending a weekend and falling in love witht the city</t>
+  </si>
+  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -316,6 +418,9 @@
     <t>jack stl</t>
   </si>
   <si>
+    <t>how he found peace after seeing the sun and books and listening to music in the library</t>
+  </si>
+  <si>
     <t>Rudy</t>
   </si>
   <si>
@@ -325,6 +430,9 @@
     <t>rudy stl</t>
   </si>
   <si>
+    <t>meeting their friend at a dog park and how they work at apple after meeting this new friend</t>
+  </si>
+  <si>
     <t>Maivi (former BFA)</t>
   </si>
   <si>
@@ -334,6 +442,9 @@
     <t xml:space="preserve">maivi stl </t>
   </si>
   <si>
+    <t>fond memories in the japanese friendship garden with her father and boyfriend and how they are fond of the plants</t>
+  </si>
+  <si>
     <t>Thanthao (former BFA)</t>
   </si>
   <si>
@@ -343,6 +454,9 @@
     <t>thanthao stl</t>
   </si>
   <si>
+    <t>Sj being a bubble of diversity with lots of different food, cultures, and activities</t>
+  </si>
+  <si>
     <t>Elham (former BA)</t>
   </si>
   <si>
@@ -352,6 +466,9 @@
     <t xml:space="preserve">elham stl </t>
   </si>
   <si>
+    <t>SJ is a welcoming city and how it feels like home and there is always something new to explore</t>
+  </si>
+  <si>
     <t>George</t>
   </si>
   <si>
@@ -361,6 +478,9 @@
     <t>george stl</t>
   </si>
   <si>
+    <t>Moved to SJ from Miami and enjoys the delicious food although he misses home, he feels welcomed here</t>
+  </si>
+  <si>
     <t>Veronica</t>
   </si>
   <si>
@@ -370,6 +490,9 @@
     <t>veronica stl</t>
   </si>
   <si>
+    <t>Moved to Sj from east coast and saw the beautiful history of the 1st mayor's home (adobe house)</t>
+  </si>
+  <si>
     <t>Ed</t>
   </si>
   <si>
@@ -377,6 +500,9 @@
   </si>
   <si>
     <t>ed stl</t>
+  </si>
+  <si>
+    <t>Used to live on Fast lance south on 280 &amp; Porter (now called Leigh &amp; 280)</t>
   </si>
   <si>
     <t>Valerie (former BFA?)</t>
@@ -392,7 +518,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -418,6 +544,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -454,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -476,13 +608,16 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -703,6 +838,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="17.0"/>
     <col customWidth="1" min="2" max="2" width="28.5"/>
+    <col customWidth="1" min="6" max="6" width="72.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -721,13 +857,19 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6">
         <v>-121.886</v>
@@ -736,15 +878,18 @@
         <v>37.338</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6">
         <v>-122.0575</v>
@@ -753,15 +898,18 @@
         <v>37.3875</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" s="6">
         <v>-121.844313</v>
@@ -770,15 +918,18 @@
         <v>37.339814</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6">
         <v>-121.894317</v>
@@ -787,15 +938,19 @@
         <v>37.336662</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6">
         <v>-121.889786</v>
@@ -804,15 +959,18 @@
         <v>37.33254</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6">
         <v>-121.890435</v>
@@ -821,32 +979,38 @@
         <v>37.336091</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6">
         <v>-121.88323</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <v>37.338477</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C9" s="6">
         <v>-121.890435</v>
@@ -855,15 +1019,18 @@
         <v>37.336091</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="C10" s="6">
         <v>-121.890435</v>
@@ -872,15 +1039,18 @@
         <v>37.336091</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6">
         <v>-121.889967</v>
@@ -889,15 +1059,18 @@
         <v>37.333956</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C12" s="6">
         <v>-121.820494</v>
@@ -906,15 +1079,18 @@
         <v>37.336519</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C13" s="6">
         <v>-121.886494</v>
@@ -923,15 +1099,18 @@
         <v>37.34878</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6">
         <v>-121.862352</v>
@@ -940,15 +1119,18 @@
         <v>37.320639</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6">
         <v>-121.890435</v>
@@ -957,15 +1139,18 @@
         <v>37.336091</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
+        <v>58</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C16" s="6">
         <v>-121.892581057239</v>
@@ -974,21 +1159,24 @@
         <v>37.3321692066064</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6">
         <v>-121.890435</v>
@@ -997,13 +1185,16 @@
         <v>37.336091</v>
       </c>
       <c r="E17" s="4"/>
+      <c r="F17" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C18" s="6">
         <v>-121.890435</v>
@@ -1012,15 +1203,18 @@
         <v>37.336091</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C19" s="6">
         <v>-121.889965</v>
@@ -1029,15 +1223,18 @@
         <v>37.336499</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C20" s="6">
         <v>-121.860026</v>
@@ -1046,15 +1243,18 @@
         <v>37.286143</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C21" s="6">
         <v>-121.886836</v>
@@ -1063,15 +1263,18 @@
         <v>37.351543</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C22" s="6">
         <v>-121.890435</v>
@@ -1080,15 +1283,18 @@
         <v>37.336091</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>63</v>
+        <v>85</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="C23" s="6">
         <v>-121.885063</v>
@@ -1097,15 +1303,18 @@
         <v>37.335661</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>66</v>
+        <v>89</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C24" s="6">
         <v>-122.142211</v>
@@ -1114,15 +1323,18 @@
         <v>37.429394</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>69</v>
+        <v>93</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C25" s="6">
         <v>-121.886473</v>
@@ -1131,15 +1343,18 @@
         <v>37.345732</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>72</v>
+        <v>97</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C26" s="6">
         <v>-121.8898206</v>
@@ -1148,15 +1363,18 @@
         <v>37.332664</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>75</v>
+        <v>101</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6">
         <v>-121.886836</v>
@@ -1165,15 +1383,18 @@
         <v>37.351543</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>77</v>
+        <v>104</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C28" s="6">
         <v>-121.8864</v>
@@ -1182,15 +1403,18 @@
         <v>37.330514</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>80</v>
+        <v>108</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C29" s="6">
         <v>-121.875582</v>
@@ -1199,21 +1423,24 @@
         <v>37.333207</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>85</v>
+        <v>112</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="C30" s="6">
         <v>-121.881092</v>
@@ -1222,15 +1449,18 @@
         <v>37.335383</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>88</v>
+        <v>118</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="C31" s="6">
         <v>-121.880996</v>
@@ -1239,15 +1469,18 @@
         <v>37.335409</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>91</v>
+        <v>122</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C32" s="6">
         <v>-121.890182</v>
@@ -1256,15 +1489,18 @@
         <v>37.33169</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>94</v>
+        <v>126</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="C33" s="6">
         <v>-121.885462</v>
@@ -1273,15 +1509,18 @@
         <v>37.357547</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>97</v>
+        <v>130</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="C34" s="6">
         <v>-121.88501</v>
@@ -1290,15 +1529,18 @@
         <v>37.335687</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>100</v>
+        <v>134</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="C35" s="6">
         <v>-121.898366</v>
@@ -1307,15 +1549,18 @@
         <v>37.342133</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>103</v>
+        <v>138</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="C36" s="6">
         <v>-121.85994</v>
@@ -1324,32 +1569,38 @@
         <v>37.322106</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>106</v>
+        <v>142</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>108</v>
+        <v>145</v>
       </c>
       <c r="C37" s="6">
         <v>-121.771485</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="8">
         <v>37.317161</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>109</v>
+        <v>146</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C38" s="6">
         <v>-121.8864</v>
@@ -1358,15 +1609,18 @@
         <v>37.330514</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>112</v>
+        <v>150</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="C39" s="6">
         <v>-121.996804</v>
@@ -1375,15 +1629,18 @@
         <v>37.306851</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>115</v>
+        <v>154</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="C40" s="6">
         <v>-121.894841</v>
@@ -1392,15 +1649,18 @@
         <v>37.337083</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>118</v>
+        <v>158</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="C41" s="6">
         <v>-121.927198</v>
@@ -1409,18 +1669,21 @@
         <v>37.314905</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>121</v>
+        <v>162</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>124</v>
+        <v>165</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="43">

</xml_diff>